<commit_message>
Actualización de usuarios.xlsx con nuevos datos
</commit_message>
<xml_diff>
--- a/usuarios.xlsx
+++ b/usuarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\nabep\WEB\credenciales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B35883DC-EE22-45B0-B846-BF9E87FF3979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A18422B8-593C-486B-9854-2A7C9F1534D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="438">
   <si>
     <t>usuario</t>
   </si>
@@ -39,9 +39,6 @@
     <t>contraseña</t>
   </si>
   <si>
-    <t>op_numero2</t>
-  </si>
-  <si>
     <t>op_numero3</t>
   </si>
   <si>
@@ -1339,6 +1336,15 @@
   </si>
   <si>
     <t>/*dK87s12P</t>
+  </si>
+  <si>
+    <t>op_anderson</t>
+  </si>
+  <si>
+    <t>Anderson</t>
+  </si>
+  <si>
+    <t>Parra</t>
   </si>
 </sst>
 </file>
@@ -1659,7 +1665,7 @@
   <dimension ref="A1:D216"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1676,1736 +1682,1742 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>431</v>
+      </c>
+      <c r="D1" t="s">
         <v>432</v>
-      </c>
-      <c r="D1" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>428</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>429</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>430</v>
-      </c>
-      <c r="D2" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>435</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>436</v>
+      </c>
+      <c r="D3" t="s">
+        <v>437</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
         <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
         <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
         <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
         <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
         <v>15</v>
-      </c>
-      <c r="B9" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
         <v>17</v>
-      </c>
-      <c r="B10" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
         <v>19</v>
-      </c>
-      <c r="B11" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
         <v>21</v>
-      </c>
-      <c r="B12" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
         <v>23</v>
-      </c>
-      <c r="B13" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" t="s">
         <v>25</v>
-      </c>
-      <c r="B14" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
         <v>27</v>
-      </c>
-      <c r="B15" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" t="s">
         <v>29</v>
-      </c>
-      <c r="B16" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" t="s">
         <v>31</v>
-      </c>
-      <c r="B17" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" t="s">
         <v>33</v>
-      </c>
-      <c r="B18" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" t="s">
         <v>35</v>
-      </c>
-      <c r="B19" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" t="s">
         <v>37</v>
-      </c>
-      <c r="B20" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" t="s">
         <v>39</v>
-      </c>
-      <c r="B21" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" t="s">
         <v>41</v>
-      </c>
-      <c r="B22" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" t="s">
         <v>43</v>
-      </c>
-      <c r="B23" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" t="s">
         <v>45</v>
-      </c>
-      <c r="B24" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" t="s">
         <v>47</v>
-      </c>
-      <c r="B25" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" t="s">
         <v>49</v>
-      </c>
-      <c r="B26" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" t="s">
         <v>51</v>
-      </c>
-      <c r="B27" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" t="s">
         <v>53</v>
-      </c>
-      <c r="B28" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" t="s">
         <v>55</v>
-      </c>
-      <c r="B29" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" t="s">
         <v>57</v>
-      </c>
-      <c r="B30" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" t="s">
         <v>59</v>
-      </c>
-      <c r="B31" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32" t="s">
         <v>61</v>
-      </c>
-      <c r="B32" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33" t="s">
         <v>63</v>
-      </c>
-      <c r="B33" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
+        <v>64</v>
+      </c>
+      <c r="B34" t="s">
         <v>65</v>
-      </c>
-      <c r="B34" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
+        <v>66</v>
+      </c>
+      <c r="B35" t="s">
         <v>67</v>
-      </c>
-      <c r="B35" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
+        <v>68</v>
+      </c>
+      <c r="B36" t="s">
         <v>69</v>
-      </c>
-      <c r="B36" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
+        <v>70</v>
+      </c>
+      <c r="B37" t="s">
         <v>71</v>
-      </c>
-      <c r="B37" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
+        <v>72</v>
+      </c>
+      <c r="B38" t="s">
         <v>73</v>
-      </c>
-      <c r="B38" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
+        <v>74</v>
+      </c>
+      <c r="B39" t="s">
         <v>75</v>
-      </c>
-      <c r="B39" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
+        <v>76</v>
+      </c>
+      <c r="B40" t="s">
         <v>77</v>
-      </c>
-      <c r="B40" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
+        <v>78</v>
+      </c>
+      <c r="B41" t="s">
         <v>79</v>
-      </c>
-      <c r="B41" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
+        <v>80</v>
+      </c>
+      <c r="B42" t="s">
         <v>81</v>
-      </c>
-      <c r="B42" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
+        <v>82</v>
+      </c>
+      <c r="B43" t="s">
         <v>83</v>
-      </c>
-      <c r="B43" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
+        <v>84</v>
+      </c>
+      <c r="B44" t="s">
         <v>85</v>
-      </c>
-      <c r="B44" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
+        <v>86</v>
+      </c>
+      <c r="B45" t="s">
         <v>87</v>
-      </c>
-      <c r="B45" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
+        <v>88</v>
+      </c>
+      <c r="B46" t="s">
         <v>89</v>
-      </c>
-      <c r="B46" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
+        <v>90</v>
+      </c>
+      <c r="B47" t="s">
         <v>91</v>
-      </c>
-      <c r="B47" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
+        <v>92</v>
+      </c>
+      <c r="B48" t="s">
         <v>93</v>
-      </c>
-      <c r="B48" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
+        <v>94</v>
+      </c>
+      <c r="B49" t="s">
         <v>95</v>
-      </c>
-      <c r="B49" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
+        <v>96</v>
+      </c>
+      <c r="B50" t="s">
         <v>97</v>
-      </c>
-      <c r="B50" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
+        <v>98</v>
+      </c>
+      <c r="B51" t="s">
         <v>99</v>
-      </c>
-      <c r="B51" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
+        <v>100</v>
+      </c>
+      <c r="B52" t="s">
         <v>101</v>
-      </c>
-      <c r="B52" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
+        <v>102</v>
+      </c>
+      <c r="B53" t="s">
         <v>103</v>
-      </c>
-      <c r="B53" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
+        <v>104</v>
+      </c>
+      <c r="B54" t="s">
         <v>105</v>
-      </c>
-      <c r="B54" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
+        <v>106</v>
+      </c>
+      <c r="B55" t="s">
         <v>107</v>
-      </c>
-      <c r="B55" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
+        <v>108</v>
+      </c>
+      <c r="B56" t="s">
         <v>109</v>
-      </c>
-      <c r="B56" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
+        <v>110</v>
+      </c>
+      <c r="B57" t="s">
         <v>111</v>
-      </c>
-      <c r="B57" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
+        <v>112</v>
+      </c>
+      <c r="B58" t="s">
         <v>113</v>
-      </c>
-      <c r="B58" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
+        <v>114</v>
+      </c>
+      <c r="B59" t="s">
         <v>115</v>
-      </c>
-      <c r="B59" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
+        <v>116</v>
+      </c>
+      <c r="B60" t="s">
         <v>117</v>
-      </c>
-      <c r="B60" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
+        <v>118</v>
+      </c>
+      <c r="B61" t="s">
         <v>119</v>
-      </c>
-      <c r="B61" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
+        <v>120</v>
+      </c>
+      <c r="B62" t="s">
         <v>121</v>
-      </c>
-      <c r="B62" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
+        <v>122</v>
+      </c>
+      <c r="B63" t="s">
         <v>123</v>
-      </c>
-      <c r="B63" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
+        <v>124</v>
+      </c>
+      <c r="B64" t="s">
         <v>125</v>
-      </c>
-      <c r="B64" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
+        <v>126</v>
+      </c>
+      <c r="B65" t="s">
         <v>127</v>
-      </c>
-      <c r="B65" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
+        <v>128</v>
+      </c>
+      <c r="B66" t="s">
         <v>129</v>
-      </c>
-      <c r="B66" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
+        <v>130</v>
+      </c>
+      <c r="B67" t="s">
         <v>131</v>
-      </c>
-      <c r="B67" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
+        <v>132</v>
+      </c>
+      <c r="B68" t="s">
         <v>133</v>
-      </c>
-      <c r="B68" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
+        <v>134</v>
+      </c>
+      <c r="B69" t="s">
         <v>135</v>
-      </c>
-      <c r="B69" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
+        <v>136</v>
+      </c>
+      <c r="B70" t="s">
         <v>137</v>
-      </c>
-      <c r="B70" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
+        <v>138</v>
+      </c>
+      <c r="B71" t="s">
         <v>139</v>
-      </c>
-      <c r="B71" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
+        <v>140</v>
+      </c>
+      <c r="B72" t="s">
         <v>141</v>
-      </c>
-      <c r="B72" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
+        <v>142</v>
+      </c>
+      <c r="B73" t="s">
         <v>143</v>
-      </c>
-      <c r="B73" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
+        <v>144</v>
+      </c>
+      <c r="B74" t="s">
         <v>145</v>
-      </c>
-      <c r="B74" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
+        <v>146</v>
+      </c>
+      <c r="B75" t="s">
         <v>147</v>
-      </c>
-      <c r="B75" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
+        <v>148</v>
+      </c>
+      <c r="B76" t="s">
         <v>149</v>
-      </c>
-      <c r="B76" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
+        <v>150</v>
+      </c>
+      <c r="B77" t="s">
         <v>151</v>
-      </c>
-      <c r="B77" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
+        <v>152</v>
+      </c>
+      <c r="B78" t="s">
         <v>153</v>
-      </c>
-      <c r="B78" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
+        <v>154</v>
+      </c>
+      <c r="B79" t="s">
         <v>155</v>
-      </c>
-      <c r="B79" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
+        <v>156</v>
+      </c>
+      <c r="B80" t="s">
         <v>157</v>
-      </c>
-      <c r="B80" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
+        <v>158</v>
+      </c>
+      <c r="B81" t="s">
         <v>159</v>
-      </c>
-      <c r="B81" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B82" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
+        <v>161</v>
+      </c>
+      <c r="B83" t="s">
         <v>162</v>
-      </c>
-      <c r="B83" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
+        <v>163</v>
+      </c>
+      <c r="B84" t="s">
         <v>164</v>
-      </c>
-      <c r="B84" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
+        <v>165</v>
+      </c>
+      <c r="B85" t="s">
         <v>166</v>
-      </c>
-      <c r="B85" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
+        <v>167</v>
+      </c>
+      <c r="B86" t="s">
         <v>168</v>
-      </c>
-      <c r="B86" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
+        <v>169</v>
+      </c>
+      <c r="B87" t="s">
         <v>170</v>
-      </c>
-      <c r="B87" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
+        <v>171</v>
+      </c>
+      <c r="B88" t="s">
         <v>172</v>
-      </c>
-      <c r="B88" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
+        <v>173</v>
+      </c>
+      <c r="B89" t="s">
         <v>174</v>
-      </c>
-      <c r="B89" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
+        <v>175</v>
+      </c>
+      <c r="B90" t="s">
         <v>176</v>
-      </c>
-      <c r="B90" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
+        <v>177</v>
+      </c>
+      <c r="B91" t="s">
         <v>178</v>
-      </c>
-      <c r="B91" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
+        <v>179</v>
+      </c>
+      <c r="B92" t="s">
         <v>180</v>
-      </c>
-      <c r="B92" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
+        <v>181</v>
+      </c>
+      <c r="B93" t="s">
         <v>182</v>
-      </c>
-      <c r="B93" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
+        <v>183</v>
+      </c>
+      <c r="B94" t="s">
         <v>184</v>
-      </c>
-      <c r="B94" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
+        <v>185</v>
+      </c>
+      <c r="B95" t="s">
         <v>186</v>
-      </c>
-      <c r="B95" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
+        <v>187</v>
+      </c>
+      <c r="B96" t="s">
         <v>188</v>
-      </c>
-      <c r="B96" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
+        <v>189</v>
+      </c>
+      <c r="B97" t="s">
         <v>190</v>
-      </c>
-      <c r="B97" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
+        <v>191</v>
+      </c>
+      <c r="B98" t="s">
         <v>192</v>
-      </c>
-      <c r="B98" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
+        <v>193</v>
+      </c>
+      <c r="B99" t="s">
         <v>194</v>
-      </c>
-      <c r="B99" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
+        <v>195</v>
+      </c>
+      <c r="B100" t="s">
         <v>196</v>
-      </c>
-      <c r="B100" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
+        <v>197</v>
+      </c>
+      <c r="B101" t="s">
         <v>198</v>
-      </c>
-      <c r="B101" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
+        <v>199</v>
+      </c>
+      <c r="B102" t="s">
         <v>200</v>
-      </c>
-      <c r="B102" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
+        <v>201</v>
+      </c>
+      <c r="B103" t="s">
         <v>202</v>
-      </c>
-      <c r="B103" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
+        <v>203</v>
+      </c>
+      <c r="B104" t="s">
         <v>204</v>
-      </c>
-      <c r="B104" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
+        <v>205</v>
+      </c>
+      <c r="B105" t="s">
         <v>206</v>
-      </c>
-      <c r="B105" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
+        <v>207</v>
+      </c>
+      <c r="B106" t="s">
         <v>208</v>
-      </c>
-      <c r="B106" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
+        <v>209</v>
+      </c>
+      <c r="B107" t="s">
         <v>210</v>
-      </c>
-      <c r="B107" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
+        <v>211</v>
+      </c>
+      <c r="B108" t="s">
         <v>212</v>
-      </c>
-      <c r="B108" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
+        <v>213</v>
+      </c>
+      <c r="B109" t="s">
         <v>214</v>
-      </c>
-      <c r="B109" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
+        <v>215</v>
+      </c>
+      <c r="B110" t="s">
         <v>216</v>
-      </c>
-      <c r="B110" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
+        <v>217</v>
+      </c>
+      <c r="B111" t="s">
         <v>218</v>
-      </c>
-      <c r="B111" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
+        <v>219</v>
+      </c>
+      <c r="B112" t="s">
         <v>220</v>
-      </c>
-      <c r="B112" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
+        <v>221</v>
+      </c>
+      <c r="B113" t="s">
         <v>222</v>
-      </c>
-      <c r="B113" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
+        <v>223</v>
+      </c>
+      <c r="B114" t="s">
         <v>224</v>
-      </c>
-      <c r="B114" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
+        <v>225</v>
+      </c>
+      <c r="B115" t="s">
         <v>226</v>
-      </c>
-      <c r="B115" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
+        <v>227</v>
+      </c>
+      <c r="B116" t="s">
         <v>228</v>
-      </c>
-      <c r="B116" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
+        <v>229</v>
+      </c>
+      <c r="B117" t="s">
         <v>230</v>
-      </c>
-      <c r="B117" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
+        <v>231</v>
+      </c>
+      <c r="B118" t="s">
         <v>232</v>
-      </c>
-      <c r="B118" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
+        <v>233</v>
+      </c>
+      <c r="B119" t="s">
         <v>234</v>
-      </c>
-      <c r="B119" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
+        <v>235</v>
+      </c>
+      <c r="B120" t="s">
         <v>236</v>
-      </c>
-      <c r="B120" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
+        <v>237</v>
+      </c>
+      <c r="B121" t="s">
         <v>238</v>
-      </c>
-      <c r="B121" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
+        <v>239</v>
+      </c>
+      <c r="B122" t="s">
         <v>240</v>
-      </c>
-      <c r="B122" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
+        <v>241</v>
+      </c>
+      <c r="B123" t="s">
         <v>242</v>
-      </c>
-      <c r="B123" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
+        <v>243</v>
+      </c>
+      <c r="B124" t="s">
         <v>244</v>
-      </c>
-      <c r="B124" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
+        <v>245</v>
+      </c>
+      <c r="B125" t="s">
         <v>246</v>
-      </c>
-      <c r="B125" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
+        <v>247</v>
+      </c>
+      <c r="B126" t="s">
         <v>248</v>
-      </c>
-      <c r="B126" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
+        <v>249</v>
+      </c>
+      <c r="B127" t="s">
         <v>250</v>
-      </c>
-      <c r="B127" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
+        <v>251</v>
+      </c>
+      <c r="B128" t="s">
         <v>252</v>
-      </c>
-      <c r="B128" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
+        <v>253</v>
+      </c>
+      <c r="B129" t="s">
         <v>254</v>
-      </c>
-      <c r="B129" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
+        <v>255</v>
+      </c>
+      <c r="B130" t="s">
         <v>256</v>
-      </c>
-      <c r="B130" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B131" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
+        <v>258</v>
+      </c>
+      <c r="B132" t="s">
         <v>259</v>
-      </c>
-      <c r="B132" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
+        <v>260</v>
+      </c>
+      <c r="B133" t="s">
         <v>261</v>
-      </c>
-      <c r="B133" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B134" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
+        <v>263</v>
+      </c>
+      <c r="B135" t="s">
         <v>264</v>
-      </c>
-      <c r="B135" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
+        <v>265</v>
+      </c>
+      <c r="B136" t="s">
         <v>266</v>
-      </c>
-      <c r="B136" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
+        <v>267</v>
+      </c>
+      <c r="B137" t="s">
         <v>268</v>
-      </c>
-      <c r="B137" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
+        <v>269</v>
+      </c>
+      <c r="B138" t="s">
         <v>270</v>
-      </c>
-      <c r="B138" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
+        <v>271</v>
+      </c>
+      <c r="B139" t="s">
         <v>272</v>
-      </c>
-      <c r="B139" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
+        <v>273</v>
+      </c>
+      <c r="B140" t="s">
         <v>274</v>
-      </c>
-      <c r="B140" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
+        <v>275</v>
+      </c>
+      <c r="B141" t="s">
         <v>276</v>
-      </c>
-      <c r="B141" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
+        <v>277</v>
+      </c>
+      <c r="B142" t="s">
         <v>278</v>
-      </c>
-      <c r="B142" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
+        <v>279</v>
+      </c>
+      <c r="B143" t="s">
         <v>280</v>
-      </c>
-      <c r="B143" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
+        <v>281</v>
+      </c>
+      <c r="B144" t="s">
         <v>282</v>
-      </c>
-      <c r="B144" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
+        <v>283</v>
+      </c>
+      <c r="B145" t="s">
         <v>284</v>
-      </c>
-      <c r="B145" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
+        <v>285</v>
+      </c>
+      <c r="B146" t="s">
         <v>286</v>
-      </c>
-      <c r="B146" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
+        <v>287</v>
+      </c>
+      <c r="B147" t="s">
         <v>288</v>
-      </c>
-      <c r="B147" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
+        <v>289</v>
+      </c>
+      <c r="B148" t="s">
         <v>290</v>
-      </c>
-      <c r="B148" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
+        <v>291</v>
+      </c>
+      <c r="B149" t="s">
         <v>292</v>
-      </c>
-      <c r="B149" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
+        <v>293</v>
+      </c>
+      <c r="B150" t="s">
         <v>294</v>
-      </c>
-      <c r="B150" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
+        <v>295</v>
+      </c>
+      <c r="B151" t="s">
         <v>296</v>
-      </c>
-      <c r="B151" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
+        <v>297</v>
+      </c>
+      <c r="B152" t="s">
         <v>298</v>
-      </c>
-      <c r="B152" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
+        <v>299</v>
+      </c>
+      <c r="B153" t="s">
         <v>300</v>
-      </c>
-      <c r="B153" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
+        <v>301</v>
+      </c>
+      <c r="B154" t="s">
         <v>302</v>
-      </c>
-      <c r="B154" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
+        <v>303</v>
+      </c>
+      <c r="B155" t="s">
         <v>304</v>
-      </c>
-      <c r="B155" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
+        <v>305</v>
+      </c>
+      <c r="B156" t="s">
         <v>306</v>
-      </c>
-      <c r="B156" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
+        <v>307</v>
+      </c>
+      <c r="B157" t="s">
         <v>308</v>
-      </c>
-      <c r="B157" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
+        <v>309</v>
+      </c>
+      <c r="B158" t="s">
         <v>310</v>
-      </c>
-      <c r="B158" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
+        <v>311</v>
+      </c>
+      <c r="B159" t="s">
         <v>312</v>
-      </c>
-      <c r="B159" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
+        <v>313</v>
+      </c>
+      <c r="B160" t="s">
         <v>314</v>
-      </c>
-      <c r="B160" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
+        <v>315</v>
+      </c>
+      <c r="B161" t="s">
         <v>316</v>
-      </c>
-      <c r="B161" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
+        <v>317</v>
+      </c>
+      <c r="B162" t="s">
         <v>318</v>
-      </c>
-      <c r="B162" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
+        <v>319</v>
+      </c>
+      <c r="B163" t="s">
         <v>320</v>
-      </c>
-      <c r="B163" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
+        <v>321</v>
+      </c>
+      <c r="B164" t="s">
         <v>322</v>
-      </c>
-      <c r="B164" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
+        <v>323</v>
+      </c>
+      <c r="B165" t="s">
         <v>324</v>
-      </c>
-      <c r="B165" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
+        <v>325</v>
+      </c>
+      <c r="B166" t="s">
         <v>326</v>
-      </c>
-      <c r="B166" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
+        <v>327</v>
+      </c>
+      <c r="B167" t="s">
         <v>328</v>
-      </c>
-      <c r="B167" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
+        <v>329</v>
+      </c>
+      <c r="B168" t="s">
         <v>330</v>
-      </c>
-      <c r="B168" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
+        <v>331</v>
+      </c>
+      <c r="B169" t="s">
         <v>332</v>
-      </c>
-      <c r="B169" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
+        <v>333</v>
+      </c>
+      <c r="B170" t="s">
         <v>334</v>
-      </c>
-      <c r="B170" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
+        <v>335</v>
+      </c>
+      <c r="B171" t="s">
         <v>336</v>
-      </c>
-      <c r="B171" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
+        <v>337</v>
+      </c>
+      <c r="B172" t="s">
         <v>338</v>
-      </c>
-      <c r="B172" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
+        <v>339</v>
+      </c>
+      <c r="B173" t="s">
         <v>340</v>
-      </c>
-      <c r="B173" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
+        <v>341</v>
+      </c>
+      <c r="B174" t="s">
         <v>342</v>
-      </c>
-      <c r="B174" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
+        <v>343</v>
+      </c>
+      <c r="B175" t="s">
         <v>344</v>
-      </c>
-      <c r="B175" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
+        <v>345</v>
+      </c>
+      <c r="B176" t="s">
         <v>346</v>
-      </c>
-      <c r="B176" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
+        <v>347</v>
+      </c>
+      <c r="B177" t="s">
         <v>348</v>
-      </c>
-      <c r="B177" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
+        <v>349</v>
+      </c>
+      <c r="B178" t="s">
         <v>350</v>
-      </c>
-      <c r="B178" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
+        <v>351</v>
+      </c>
+      <c r="B179" t="s">
         <v>352</v>
-      </c>
-      <c r="B179" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
+        <v>353</v>
+      </c>
+      <c r="B180" t="s">
         <v>354</v>
-      </c>
-      <c r="B180" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
+        <v>355</v>
+      </c>
+      <c r="B181" t="s">
         <v>356</v>
-      </c>
-      <c r="B181" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
+        <v>357</v>
+      </c>
+      <c r="B182" t="s">
         <v>358</v>
-      </c>
-      <c r="B182" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
+        <v>359</v>
+      </c>
+      <c r="B183" t="s">
         <v>360</v>
-      </c>
-      <c r="B183" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
+        <v>361</v>
+      </c>
+      <c r="B184" t="s">
         <v>362</v>
-      </c>
-      <c r="B184" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
+        <v>363</v>
+      </c>
+      <c r="B185" t="s">
         <v>364</v>
-      </c>
-      <c r="B185" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
+        <v>365</v>
+      </c>
+      <c r="B186" t="s">
         <v>366</v>
-      </c>
-      <c r="B186" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
+        <v>367</v>
+      </c>
+      <c r="B187" t="s">
         <v>368</v>
-      </c>
-      <c r="B187" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
+        <v>369</v>
+      </c>
+      <c r="B188" t="s">
         <v>370</v>
-      </c>
-      <c r="B188" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
+        <v>371</v>
+      </c>
+      <c r="B189" t="s">
         <v>372</v>
-      </c>
-      <c r="B189" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
+        <v>373</v>
+      </c>
+      <c r="B190" t="s">
         <v>374</v>
-      </c>
-      <c r="B190" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
+        <v>375</v>
+      </c>
+      <c r="B191" t="s">
         <v>376</v>
-      </c>
-      <c r="B191" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
+        <v>377</v>
+      </c>
+      <c r="B192" t="s">
         <v>378</v>
-      </c>
-      <c r="B192" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
+        <v>379</v>
+      </c>
+      <c r="B193" t="s">
         <v>380</v>
-      </c>
-      <c r="B193" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
+        <v>381</v>
+      </c>
+      <c r="B194" t="s">
         <v>382</v>
-      </c>
-      <c r="B194" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
+        <v>383</v>
+      </c>
+      <c r="B195" t="s">
         <v>384</v>
-      </c>
-      <c r="B195" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
+        <v>385</v>
+      </c>
+      <c r="B196" t="s">
         <v>386</v>
-      </c>
-      <c r="B196" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
+        <v>387</v>
+      </c>
+      <c r="B197" t="s">
         <v>388</v>
-      </c>
-      <c r="B197" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
+        <v>389</v>
+      </c>
+      <c r="B198" t="s">
         <v>390</v>
-      </c>
-      <c r="B198" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
+        <v>391</v>
+      </c>
+      <c r="B199" t="s">
         <v>392</v>
-      </c>
-      <c r="B199" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B200" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
+        <v>394</v>
+      </c>
+      <c r="B201" t="s">
         <v>395</v>
-      </c>
-      <c r="B201" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
+        <v>396</v>
+      </c>
+      <c r="B202" t="s">
         <v>397</v>
-      </c>
-      <c r="B202" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
+        <v>398</v>
+      </c>
+      <c r="B203" t="s">
         <v>399</v>
-      </c>
-      <c r="B203" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
+        <v>400</v>
+      </c>
+      <c r="B204" t="s">
         <v>401</v>
-      </c>
-      <c r="B204" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
+        <v>402</v>
+      </c>
+      <c r="B205" t="s">
         <v>403</v>
-      </c>
-      <c r="B205" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
+        <v>404</v>
+      </c>
+      <c r="B206" t="s">
         <v>405</v>
-      </c>
-      <c r="B206" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
+        <v>406</v>
+      </c>
+      <c r="B207" t="s">
         <v>407</v>
-      </c>
-      <c r="B207" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
+        <v>408</v>
+      </c>
+      <c r="B208" t="s">
         <v>409</v>
-      </c>
-      <c r="B208" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
+        <v>410</v>
+      </c>
+      <c r="B209" t="s">
         <v>411</v>
-      </c>
-      <c r="B209" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
+        <v>412</v>
+      </c>
+      <c r="B210" t="s">
         <v>413</v>
-      </c>
-      <c r="B210" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
+        <v>414</v>
+      </c>
+      <c r="B211" t="s">
         <v>415</v>
-      </c>
-      <c r="B211" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
+        <v>416</v>
+      </c>
+      <c r="B212" t="s">
         <v>417</v>
-      </c>
-      <c r="B212" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
+        <v>418</v>
+      </c>
+      <c r="B213" t="s">
         <v>419</v>
-      </c>
-      <c r="B213" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
+        <v>420</v>
+      </c>
+      <c r="B214" t="s">
         <v>421</v>
-      </c>
-      <c r="B214" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
+        <v>422</v>
+      </c>
+      <c r="B215" t="s">
         <v>423</v>
-      </c>
-      <c r="B215" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
+        <v>424</v>
+      </c>
+      <c r="B216" t="s">
         <v>425</v>
-      </c>
-      <c r="B216" t="s">
-        <v>426</v>
       </c>
     </row>
   </sheetData>

</xml_diff>